<commit_message>
passed the dataframe to a file using a function
</commit_message>
<xml_diff>
--- a/a-results2.xlsx
+++ b/a-results2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,46 +507,46 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15615</v>
+        <v>15613</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Heri Dati</t>
+          <t>Steve Coup</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D2" t="n">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="E2" t="n">
+        <v>68</v>
+      </c>
+      <c r="F2" t="n">
+        <v>48</v>
+      </c>
+      <c r="G2" t="n">
+        <v>70</v>
+      </c>
+      <c r="H2" t="n">
+        <v>81</v>
+      </c>
+      <c r="I2" t="n">
+        <v>54</v>
+      </c>
+      <c r="J2" t="n">
         <v>89</v>
       </c>
-      <c r="F2" t="n">
-        <v>79</v>
-      </c>
-      <c r="G2" t="n">
-        <v>80</v>
-      </c>
-      <c r="H2" t="n">
-        <v>86</v>
-      </c>
-      <c r="I2" t="n">
-        <v>90</v>
-      </c>
-      <c r="J2" t="n">
-        <v>87</v>
-      </c>
       <c r="K2" t="n">
-        <v>679</v>
+        <v>534</v>
       </c>
       <c r="L2" t="n">
-        <v>84.875</v>
+        <v>66.75</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>A-</t>
+          <t>B-</t>
         </is>
       </c>
       <c r="N2" t="n">
@@ -563,38 +563,38 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="D3" t="n">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E3" t="n">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="F3" t="n">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="G3" t="n">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="H3" t="n">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="I3" t="n">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="J3" t="n">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="K3" t="n">
-        <v>610</v>
+        <v>531</v>
       </c>
       <c r="L3" t="n">
-        <v>76.25</v>
+        <v>66.375</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>B+</t>
+          <t>B-</t>
         </is>
       </c>
       <c r="N3" t="n">
@@ -603,146 +603,50 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15613</v>
+        <v>15612</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Steve Coup</t>
+          <t>Bostwald Kite</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D4" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E4" t="n">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="F4" t="n">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="G4" t="n">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H4" t="n">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="I4" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J4" t="n">
-        <v>45</v>
+        <v>69</v>
       </c>
       <c r="K4" t="n">
-        <v>577</v>
+        <v>503</v>
       </c>
       <c r="L4" t="n">
-        <v>72.125</v>
+        <v>62.875</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>C+</t>
         </is>
       </c>
       <c r="N4" t="n">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>15612</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Bostwald Kite</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>56</v>
-      </c>
-      <c r="D5" t="n">
-        <v>78</v>
-      </c>
-      <c r="E5" t="n">
-        <v>45</v>
-      </c>
-      <c r="F5" t="n">
-        <v>78</v>
-      </c>
-      <c r="G5" t="n">
-        <v>89</v>
-      </c>
-      <c r="H5" t="n">
-        <v>56</v>
-      </c>
-      <c r="I5" t="n">
-        <v>78</v>
-      </c>
-      <c r="J5" t="n">
-        <v>90</v>
-      </c>
-      <c r="K5" t="n">
-        <v>570</v>
-      </c>
-      <c r="L5" t="n">
-        <v>71.25</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="N5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>15614</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Nderi Neti</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>76</v>
-      </c>
-      <c r="D6" t="n">
-        <v>56</v>
-      </c>
-      <c r="E6" t="n">
-        <v>76</v>
-      </c>
-      <c r="F6" t="n">
-        <v>45</v>
-      </c>
-      <c r="G6" t="n">
-        <v>67</v>
-      </c>
-      <c r="H6" t="n">
-        <v>56</v>
-      </c>
-      <c r="I6" t="n">
-        <v>78</v>
-      </c>
-      <c r="J6" t="n">
-        <v>90</v>
-      </c>
-      <c r="K6" t="n">
-        <v>544</v>
-      </c>
-      <c r="L6" t="n">
-        <v>68</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>B-</t>
-        </is>
-      </c>
-      <c r="N6" t="n">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enabled editing results of both individual and whole class at a go
</commit_message>
<xml_diff>
--- a/a-results2.xlsx
+++ b/a-results2.xlsx
@@ -521,7 +521,7 @@
         <v>44</v>
       </c>
       <c r="E2" t="n">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="F2" t="n">
         <v>48</v>
@@ -539,10 +539,10 @@
         <v>90</v>
       </c>
       <c r="K2" t="n">
-        <v>535</v>
+        <v>545</v>
       </c>
       <c r="L2" t="n">
-        <v>66.875</v>
+        <v>68.125</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -569,7 +569,7 @@
         <v>64</v>
       </c>
       <c r="E3" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="F3" t="n">
         <v>59</v>
@@ -587,10 +587,10 @@
         <v>86</v>
       </c>
       <c r="K3" t="n">
-        <v>521</v>
+        <v>541</v>
       </c>
       <c r="L3" t="n">
-        <v>65.125</v>
+        <v>67.625</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
changed how marks are entered
</commit_message>
<xml_diff>
--- a/a-results2.xlsx
+++ b/a-results2.xlsx
@@ -507,46 +507,36 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15613</v>
+        <v>15611</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Steve Coup</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>80</v>
-      </c>
+          <t>dan</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="n">
-        <v>44</v>
-      </c>
-      <c r="E2" t="n">
-        <v>78</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>48</v>
-      </c>
-      <c r="G2" t="n">
-        <v>70</v>
-      </c>
-      <c r="H2" t="n">
-        <v>81</v>
-      </c>
-      <c r="I2" t="n">
-        <v>54</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="K2" t="n">
-        <v>545</v>
+        <v>237</v>
       </c>
       <c r="L2" t="n">
-        <v>68.125</v>
+        <v>29.625</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>B-</t>
+          <t>E</t>
         </is>
       </c>
       <c r="N2" t="n">
@@ -555,46 +545,36 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>15611</v>
+        <v>15612</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fredrick Ndote</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>70</v>
-      </c>
+          <t>tes</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="n">
-        <v>64</v>
-      </c>
-      <c r="E3" t="n">
-        <v>60</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>59</v>
-      </c>
-      <c r="G3" t="n">
-        <v>90</v>
-      </c>
-      <c r="H3" t="n">
-        <v>76</v>
-      </c>
-      <c r="I3" t="n">
-        <v>36</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="K3" t="n">
-        <v>541</v>
+        <v>215</v>
       </c>
       <c r="L3" t="n">
-        <v>67.625</v>
+        <v>26.875</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>B-</t>
+          <t>E</t>
         </is>
       </c>
       <c r="N3" t="n">

</xml_diff>

<commit_message>
added rank to subjects
</commit_message>
<xml_diff>
--- a/a-results2.xlsx
+++ b/a-results2.xlsx
@@ -507,32 +507,30 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15611</v>
+        <v>15612</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dan</t>
+          <t>WER</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>87</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="n">
-        <v>74</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>89</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>78</v>
+      </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
-        <v>76</v>
-      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
-        <v>237</v>
+        <v>167</v>
       </c>
       <c r="L2" t="n">
-        <v>29.625</v>
+        <v>20.875</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -545,32 +543,30 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>15612</v>
+        <v>15611</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>tes</t>
+          <t>SAD</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>89</v>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="n">
-        <v>48</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>54</v>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>56</v>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="n">
-        <v>78</v>
-      </c>
+      <c r="J3" t="inlineStr"/>
       <c r="K3" t="n">
-        <v>215</v>
+        <v>110</v>
       </c>
       <c r="L3" t="n">
-        <v>26.875</v>
+        <v>13.75</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
changed how results are ranked
</commit_message>
<xml_diff>
--- a/a-results2.xlsx
+++ b/a-results2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,34 +507,46 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>15612</v>
+        <v>15630</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>WER</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+          <t>Balito Behil</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>92</v>
+      </c>
+      <c r="D2" t="n">
+        <v>91</v>
+      </c>
       <c r="E2" t="n">
-        <v>89</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
+        <v>88</v>
+      </c>
+      <c r="F2" t="n">
+        <v>95</v>
+      </c>
       <c r="G2" t="n">
-        <v>78</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+        <v>81</v>
+      </c>
+      <c r="H2" t="n">
+        <v>73</v>
+      </c>
+      <c r="I2" t="n">
+        <v>99</v>
+      </c>
+      <c r="J2" t="n">
+        <v>79</v>
+      </c>
       <c r="K2" t="n">
-        <v>167</v>
+        <v>698</v>
       </c>
       <c r="L2" t="n">
-        <v>20.875</v>
+        <v>87.25</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A-</t>
         </is>
       </c>
       <c r="N2" t="n">
@@ -543,38 +555,514 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>15611</v>
+        <v>15631</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SAD</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+          <t>Teti Nderi</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>72</v>
+      </c>
+      <c r="D3" t="n">
+        <v>85</v>
+      </c>
       <c r="E3" t="n">
-        <v>54</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
+        <v>92</v>
+      </c>
+      <c r="F3" t="n">
+        <v>70</v>
+      </c>
       <c r="G3" t="n">
-        <v>56</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+        <v>97</v>
+      </c>
+      <c r="H3" t="n">
+        <v>80</v>
+      </c>
+      <c r="I3" t="n">
+        <v>76</v>
+      </c>
+      <c r="J3" t="n">
+        <v>98</v>
+      </c>
       <c r="K3" t="n">
-        <v>110</v>
+        <v>670</v>
       </c>
       <c r="L3" t="n">
-        <v>13.75</v>
+        <v>83.75</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A-</t>
         </is>
       </c>
       <c r="N3" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>15628</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Seti Kitoti</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>88</v>
+      </c>
+      <c r="D4" t="n">
+        <v>69</v>
+      </c>
+      <c r="E4" t="n">
+        <v>70</v>
+      </c>
+      <c r="F4" t="n">
+        <v>65</v>
+      </c>
+      <c r="G4" t="n">
+        <v>83</v>
+      </c>
+      <c r="H4" t="n">
+        <v>77</v>
+      </c>
+      <c r="I4" t="n">
+        <v>93</v>
+      </c>
+      <c r="J4" t="n">
+        <v>67</v>
+      </c>
+      <c r="K4" t="n">
+        <v>612</v>
+      </c>
+      <c r="L4" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15625</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Bolivia Shesi</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>50</v>
+      </c>
+      <c r="D5" t="n">
+        <v>88</v>
+      </c>
+      <c r="E5" t="n">
+        <v>85</v>
+      </c>
+      <c r="F5" t="n">
+        <v>72</v>
+      </c>
+      <c r="G5" t="n">
+        <v>82</v>
+      </c>
+      <c r="H5" t="n">
+        <v>43</v>
+      </c>
+      <c r="I5" t="n">
+        <v>86</v>
+      </c>
+      <c r="J5" t="n">
+        <v>94</v>
+      </c>
+      <c r="K5" t="n">
+        <v>600</v>
+      </c>
+      <c r="L5" t="n">
+        <v>75</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>15629</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Many Matike</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>85</v>
+      </c>
+      <c r="D6" t="n">
+        <v>81</v>
+      </c>
+      <c r="E6" t="n">
+        <v>86</v>
+      </c>
+      <c r="F6" t="n">
+        <v>54</v>
+      </c>
+      <c r="G6" t="n">
+        <v>71</v>
+      </c>
+      <c r="H6" t="n">
+        <v>80</v>
+      </c>
+      <c r="I6" t="n">
+        <v>53</v>
+      </c>
+      <c r="J6" t="n">
+        <v>78</v>
+      </c>
+      <c r="K6" t="n">
+        <v>588</v>
+      </c>
+      <c r="L6" t="n">
+        <v>73.5</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>15626</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Tahmeed Ndero</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>84</v>
+      </c>
+      <c r="D7" t="n">
+        <v>51</v>
+      </c>
+      <c r="E7" t="n">
+        <v>55</v>
+      </c>
+      <c r="F7" t="n">
+        <v>63</v>
+      </c>
+      <c r="G7" t="n">
+        <v>64</v>
+      </c>
+      <c r="H7" t="n">
+        <v>86</v>
+      </c>
+      <c r="I7" t="n">
+        <v>86</v>
+      </c>
+      <c r="J7" t="n">
+        <v>89</v>
+      </c>
+      <c r="K7" t="n">
+        <v>578</v>
+      </c>
+      <c r="L7" t="n">
+        <v>72.25</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="N7" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>15627</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Dodi Biru</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>77</v>
+      </c>
+      <c r="D8" t="n">
+        <v>94</v>
+      </c>
+      <c r="E8" t="n">
+        <v>78</v>
+      </c>
+      <c r="F8" t="n">
+        <v>54</v>
+      </c>
+      <c r="G8" t="n">
+        <v>56</v>
+      </c>
+      <c r="H8" t="n">
+        <v>63</v>
+      </c>
+      <c r="I8" t="n">
+        <v>59</v>
+      </c>
+      <c r="J8" t="n">
+        <v>61</v>
+      </c>
+      <c r="K8" t="n">
+        <v>542</v>
+      </c>
+      <c r="L8" t="n">
+        <v>67.75</v>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>B-</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>15614</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Leonard Shiunde</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>69</v>
+      </c>
+      <c r="D9" t="n">
+        <v>89</v>
+      </c>
+      <c r="E9" t="n">
+        <v>54</v>
+      </c>
+      <c r="F9" t="n">
+        <v>36</v>
+      </c>
+      <c r="G9" t="n">
+        <v>80</v>
+      </c>
+      <c r="H9" t="n">
+        <v>76</v>
+      </c>
+      <c r="I9" t="n">
+        <v>80</v>
+      </c>
+      <c r="J9" t="n">
+        <v>54</v>
+      </c>
+      <c r="K9" t="n">
+        <v>538</v>
+      </c>
+      <c r="L9" t="n">
+        <v>67.25</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>B-</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>15613</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Steve Coup</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>80</v>
+      </c>
+      <c r="D10" t="n">
+        <v>44</v>
+      </c>
+      <c r="E10" t="n">
+        <v>68</v>
+      </c>
+      <c r="F10" t="n">
+        <v>48</v>
+      </c>
+      <c r="G10" t="n">
+        <v>70</v>
+      </c>
+      <c r="H10" t="n">
+        <v>81</v>
+      </c>
+      <c r="I10" t="n">
+        <v>54</v>
+      </c>
+      <c r="J10" t="n">
+        <v>89</v>
+      </c>
+      <c r="K10" t="n">
+        <v>534</v>
+      </c>
+      <c r="L10" t="n">
+        <v>66.75</v>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>B-</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>15612</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Bostwald Kite</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>56</v>
+      </c>
+      <c r="D11" t="n">
+        <v>79</v>
+      </c>
+      <c r="E11" t="n">
+        <v>36</v>
+      </c>
+      <c r="F11" t="n">
+        <v>60</v>
+      </c>
+      <c r="G11" t="n">
+        <v>87</v>
+      </c>
+      <c r="H11" t="n">
+        <v>48</v>
+      </c>
+      <c r="I11" t="n">
+        <v>68</v>
+      </c>
+      <c r="J11" t="n">
+        <v>69</v>
+      </c>
+      <c r="K11" t="n">
+        <v>503</v>
+      </c>
+      <c r="L11" t="n">
+        <v>62.875</v>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>C+</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>15632</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Cheti Nzuri</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>94</v>
+      </c>
+      <c r="D12" t="n">
+        <v>80</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>89</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
+        <v>83</v>
+      </c>
+      <c r="K12" t="n">
+        <v>346</v>
+      </c>
+      <c r="L12" t="n">
+        <v>43.25</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>15633</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Zediru Betike</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>92</v>
+      </c>
+      <c r="D13" t="n">
+        <v>82</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>90</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="n">
+        <v>81</v>
+      </c>
+      <c r="K13" t="n">
+        <v>345</v>
+      </c>
+      <c r="L13" t="n">
+        <v>43.125</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>